<commit_message>
Uso de claves foráneas para relacionar tablas
</commit_message>
<xml_diff>
--- a/MySQL/Relaciones/Relaciones.xlsx
+++ b/MySQL/Relaciones/Relaciones.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cursos\mh-curso-php8\MySQL\Relaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84A6D8-241A-453F-B7D4-0CADB04E4A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4441ED36-51C6-4501-82DF-546588FCCDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F3D2203F-EF55-4432-ACB6-E93AF3BA8781}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F3D2203F-EF55-4432-ACB6-E93AF3BA8781}"/>
   </bookViews>
   <sheets>
     <sheet name="Contactos" sheetId="1" r:id="rId1"/>
     <sheet name="Reuniones" sheetId="2" r:id="rId2"/>
-    <sheet name="Reuniones2" sheetId="3" r:id="rId3"/>
+    <sheet name="Reuniones relacionadas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>contactos_id</t>
   </si>
 </sst>
 </file>
@@ -133,8 +136,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -211,14 +214,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -537,7 +540,7 @@
   <dimension ref="B2:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,144 +551,144 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>34173</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>22391</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>35006</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>21592</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>1</v>
       </c>
     </row>
@@ -709,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260AF249-80F9-4A0A-841A-2FE949081277}">
   <dimension ref="B2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,189 +725,189 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
         <v>45730.791666666664</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>45730.791666666664</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>45730.791666608799</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>45730.791666608799</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>45730.791666608799</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -927,12 +930,286 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBB0E27-A745-4A8A-92F7-4CDCAAADF63F}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4">
+        <v>34173</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="4">
+        <v>22391</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="4">
+        <v>35006</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="4">
+        <v>21592</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45730.791666666664</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45730.791666666664</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5">
+        <v>45730.791666608799</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45767.791666666664</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>45767.791666666664</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B11:F11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{0F0F17F0-44A2-46CE-8803-5BCEE2A02C9A}"/>
+    <hyperlink ref="G6:G8" r:id="rId2" display="manuel@prueba.com" xr:uid="{EE87A2DF-13EB-4F6A-95A4-4768C26627F4}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{FED7312D-E5E5-4021-9E7B-9075859913A7}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{1BBE6E65-1821-4B79-A174-60B638FEC75D}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{447FCF73-EE2C-4568-80B9-23FD64296F73}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Relaciones entre tablas, integridad referencial y cascadas
</commit_message>
<xml_diff>
--- a/MySQL/Relaciones/Relaciones.xlsx
+++ b/MySQL/Relaciones/Relaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cursos\mh-curso-php8\MySQL\Relaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4441ED36-51C6-4501-82DF-546588FCCDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF1323-FBAD-4B31-816A-354CE7EA54D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F3D2203F-EF55-4432-ACB6-E93AF3BA8781}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F3D2203F-EF55-4432-ACB6-E93AF3BA8781}"/>
   </bookViews>
   <sheets>
     <sheet name="Contactos" sheetId="1" r:id="rId1"/>
@@ -933,7 +933,7 @@
   <dimension ref="B3:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cruces o consultas multitablas, joins
</commit_message>
<xml_diff>
--- a/MySQL/Relaciones/Relaciones.xlsx
+++ b/MySQL/Relaciones/Relaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cursos\mh-curso-php8\MySQL\Relaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF1323-FBAD-4B31-816A-354CE7EA54D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D11A1E-3B37-4E77-B241-EFC3105685C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F3D2203F-EF55-4432-ACB6-E93AF3BA8781}"/>
+    <workbookView xWindow="-20520" yWindow="2505" windowWidth="20640" windowHeight="11040" activeTab="2" xr2:uid="{F3D2203F-EF55-4432-ACB6-E93AF3BA8781}"/>
   </bookViews>
   <sheets>
     <sheet name="Contactos" sheetId="1" r:id="rId1"/>
@@ -933,7 +933,7 @@
   <dimension ref="B3:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>